<commit_message>
Cleaning on merged file
</commit_message>
<xml_diff>
--- a/Cleaning Notebooks/2015-Passouts/Merged/Cleaning.xlsx
+++ b/Cleaning Notebooks/2015-Passouts/Merged/Cleaning.xlsx
@@ -1,20 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prashant/Downloads/Student-Placement-Guidance/Cleaning Notebooks/2015-Passouts/Merged/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="15800"/>
   </bookViews>
   <sheets>
     <sheet name="Cleaning" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cleaning!$A$1:$CC$116</definedName>
+  </definedNames>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="214">
   <si>
     <t>NAME OF CANDIDATE</t>
   </si>
@@ -604,27 +620,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>1028#10</t>
-  </si>
-  <si>
-    <t>1140#10</t>
-  </si>
-  <si>
-    <t>512#10</t>
-  </si>
-  <si>
-    <t>506#10</t>
-  </si>
-  <si>
-    <t>1048#10</t>
-  </si>
-  <si>
-    <t>1094#10</t>
-  </si>
-  <si>
-    <t>496#10</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -675,12 +670,15 @@
   <si>
     <t>Praxis Technologies Ltd.</t>
   </si>
+  <si>
+    <t>Company -1/0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,7 +703,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -728,13 +726,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -743,6 +755,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -789,12 +806,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -821,14 +838,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -855,6 +873,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1030,14 +1049,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CB116"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CC116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
+      <selection activeCell="CE15" sqref="CE15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="4" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="9" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="10" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:80">
+    <row r="1" spans="1:81" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1275,8 +1375,11 @@
       <c r="CB1" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="CC1" s="2" t="s">
+        <v>213</v>
+      </c>
     </row>
-    <row r="2" spans="1:80">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1511,8 +1614,11 @@
       <c r="CA2" t="s">
         <v>195</v>
       </c>
+      <c r="CC2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:80">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1748,10 +1854,13 @@
         <v>195</v>
       </c>
       <c r="CB3" t="s">
-        <v>204</v>
+        <v>197</v>
+      </c>
+      <c r="CC3">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:80">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1909,7 +2018,7 @@
         <v>21</v>
       </c>
       <c r="BA4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB4">
         <v>23</v>
@@ -1989,8 +2098,11 @@
       <c r="CA4" t="s">
         <v>195</v>
       </c>
+      <c r="CC4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:80">
+    <row r="5" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2148,7 +2260,7 @@
         <v>23</v>
       </c>
       <c r="BA5" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB5">
         <v>22</v>
@@ -2229,10 +2341,13 @@
         <v>195</v>
       </c>
       <c r="CB5" t="s">
-        <v>205</v>
+        <v>198</v>
+      </c>
+      <c r="CC5">
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:80">
+    <row r="6" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2390,7 +2505,7 @@
         <v>20</v>
       </c>
       <c r="BA6" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB6">
         <v>21</v>
@@ -2470,8 +2585,11 @@
       <c r="CA6" t="s">
         <v>195</v>
       </c>
+      <c r="CC6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:80">
+    <row r="7" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2707,10 +2825,13 @@
         <v>195</v>
       </c>
       <c r="CB7" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC7">
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:80">
+    <row r="8" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2946,10 +3067,13 @@
         <v>195</v>
       </c>
       <c r="CB8" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC8">
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:80">
+    <row r="9" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3184,8 +3308,11 @@
       <c r="CA9" t="s">
         <v>195</v>
       </c>
+      <c r="CC9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:80">
+    <row r="10" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3234,6 +3361,9 @@
       <c r="Q10">
         <v>42</v>
       </c>
+      <c r="R10">
+        <v>419</v>
+      </c>
       <c r="S10" t="s">
         <v>195</v>
       </c>
@@ -3415,10 +3545,13 @@
         <v>195</v>
       </c>
       <c r="CB10" t="s">
-        <v>207</v>
+        <v>200</v>
+      </c>
+      <c r="CC10">
+        <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:80">
+    <row r="11" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3653,8 +3786,11 @@
       <c r="CA11" t="s">
         <v>195</v>
       </c>
+      <c r="CC11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:80">
+    <row r="12" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3812,7 +3948,7 @@
         <v>18</v>
       </c>
       <c r="BA12" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB12">
         <v>18</v>
@@ -3892,8 +4028,11 @@
       <c r="CA12" t="s">
         <v>195</v>
       </c>
+      <c r="CC12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:80">
+    <row r="13" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3942,6 +4081,9 @@
       <c r="Q13">
         <v>33</v>
       </c>
+      <c r="R13">
+        <v>394</v>
+      </c>
       <c r="S13" t="s">
         <v>195</v>
       </c>
@@ -4122,8 +4264,11 @@
       <c r="CA13" t="s">
         <v>195</v>
       </c>
+      <c r="CC13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:80">
+    <row r="14" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4358,8 +4503,11 @@
       <c r="CA14" t="s">
         <v>195</v>
       </c>
+      <c r="CC14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:80">
+    <row r="15" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4595,10 +4743,13 @@
         <v>195</v>
       </c>
       <c r="CB15" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC15">
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:80">
+    <row r="16" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4756,7 +4907,7 @@
         <v>19</v>
       </c>
       <c r="BA16" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB16">
         <v>21</v>
@@ -4836,8 +4987,11 @@
       <c r="CA16" t="s">
         <v>195</v>
       </c>
+      <c r="CC16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:80">
+    <row r="17" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -4949,8 +5103,8 @@
       <c r="AK17">
         <v>499</v>
       </c>
-      <c r="AL17" t="s">
-        <v>196</v>
+      <c r="AL17">
+        <v>1028</v>
       </c>
       <c r="AM17" t="s">
         <v>195</v>
@@ -5073,10 +5227,13 @@
         <v>195</v>
       </c>
       <c r="CB17" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC17">
+        <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:80">
+    <row r="18" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -5234,7 +5391,7 @@
         <v>22</v>
       </c>
       <c r="BA18" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB18">
         <v>19</v>
@@ -5314,8 +5471,11 @@
       <c r="CA18" t="s">
         <v>195</v>
       </c>
+      <c r="CC18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:80">
+    <row r="19" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -5551,10 +5711,13 @@
         <v>195</v>
       </c>
       <c r="CB19" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC19">
+        <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:80">
+    <row r="20" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -5790,10 +5953,13 @@
         <v>195</v>
       </c>
       <c r="CB20" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC20">
+        <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:80">
+    <row r="21" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -5948,7 +6114,7 @@
         <v>20</v>
       </c>
       <c r="BA21" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB21">
         <v>20</v>
@@ -6028,8 +6194,11 @@
       <c r="CA21" t="s">
         <v>194</v>
       </c>
+      <c r="CC21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:80">
+    <row r="22" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -6264,8 +6433,11 @@
       <c r="CA22" t="s">
         <v>195</v>
       </c>
+      <c r="CC22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:80">
+    <row r="23" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -6314,6 +6486,9 @@
       <c r="Q23">
         <v>39</v>
       </c>
+      <c r="R23">
+        <v>427</v>
+      </c>
       <c r="S23" t="s">
         <v>195</v>
       </c>
@@ -6495,10 +6670,13 @@
         <v>195</v>
       </c>
       <c r="CB23" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC23">
+        <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:80">
+    <row r="24" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -6610,8 +6788,8 @@
       <c r="AK24">
         <v>553</v>
       </c>
-      <c r="AL24" t="s">
-        <v>197</v>
+      <c r="AL24">
+        <v>1140</v>
       </c>
       <c r="AM24" t="s">
         <v>195</v>
@@ -6734,10 +6912,13 @@
         <v>195</v>
       </c>
       <c r="CB24" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC24">
+        <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:80">
+    <row r="25" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -6972,8 +7153,11 @@
       <c r="CA25" t="s">
         <v>195</v>
       </c>
+      <c r="CC25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:80">
+    <row r="26" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -7131,7 +7315,7 @@
         <v>18</v>
       </c>
       <c r="BA26" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB26">
         <v>17</v>
@@ -7211,8 +7395,11 @@
       <c r="CA26" t="s">
         <v>195</v>
       </c>
+      <c r="CC26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:80">
+    <row r="27" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -7324,8 +7511,8 @@
       <c r="AK27">
         <v>501</v>
       </c>
-      <c r="AL27" t="s">
-        <v>198</v>
+      <c r="AL27">
+        <v>512</v>
       </c>
       <c r="AM27" t="s">
         <v>195</v>
@@ -7447,8 +7634,11 @@
       <c r="CA27" t="s">
         <v>195</v>
       </c>
+      <c r="CC27">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:80">
+    <row r="28" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -7684,10 +7874,13 @@
         <v>195</v>
       </c>
       <c r="CB28" t="s">
-        <v>208</v>
+        <v>201</v>
+      </c>
+      <c r="CC28">
+        <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:80">
+    <row r="29" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -7799,8 +7992,8 @@
       <c r="AK29">
         <v>528</v>
       </c>
-      <c r="AL29" t="s">
-        <v>199</v>
+      <c r="AL29">
+        <v>506</v>
       </c>
       <c r="AM29" t="s">
         <v>195</v>
@@ -7923,10 +8116,13 @@
         <v>195</v>
       </c>
       <c r="CB29" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC29">
+        <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:80">
+    <row r="30" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -8162,10 +8358,13 @@
         <v>195</v>
       </c>
       <c r="CB30" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC30">
+        <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:80">
+    <row r="31" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -8311,7 +8510,7 @@
         <v>15</v>
       </c>
       <c r="BA31" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB31">
         <v>16</v>
@@ -8385,8 +8584,11 @@
       <c r="CA31" t="s">
         <v>194</v>
       </c>
+      <c r="CC31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:80">
+    <row r="32" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -8498,8 +8700,8 @@
       <c r="AK32">
         <v>517</v>
       </c>
-      <c r="AL32" t="s">
-        <v>200</v>
+      <c r="AL32">
+        <v>1048</v>
       </c>
       <c r="AM32" t="s">
         <v>195</v>
@@ -8621,8 +8823,11 @@
       <c r="CA32" t="s">
         <v>195</v>
       </c>
+      <c r="CC32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:80">
+    <row r="33" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -8858,10 +9063,13 @@
         <v>195</v>
       </c>
       <c r="CB33" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC33">
+        <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:80">
+    <row r="34" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -9097,10 +9305,13 @@
         <v>195</v>
       </c>
       <c r="CB34" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC34">
+        <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:80">
+    <row r="35" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -9212,8 +9423,8 @@
       <c r="AK35">
         <v>515</v>
       </c>
-      <c r="AL35" t="s">
-        <v>201</v>
+      <c r="AL35">
+        <v>1094</v>
       </c>
       <c r="AM35" t="s">
         <v>195</v>
@@ -9336,10 +9547,13 @@
         <v>195</v>
       </c>
       <c r="CB35" t="s">
-        <v>209</v>
+        <v>202</v>
+      </c>
+      <c r="CC35">
+        <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:80">
+    <row r="36" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -9575,10 +9789,13 @@
         <v>195</v>
       </c>
       <c r="CB36" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC36">
+        <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:80">
+    <row r="37" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -9814,10 +10031,13 @@
         <v>195</v>
       </c>
       <c r="CB37" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC37">
+        <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:80">
+    <row r="38" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -9975,7 +10195,7 @@
         <v>19</v>
       </c>
       <c r="BA38" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB38">
         <v>19</v>
@@ -10055,8 +10275,11 @@
       <c r="CA38" t="s">
         <v>195</v>
       </c>
+      <c r="CC38">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:80">
+    <row r="39" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -10292,10 +10515,13 @@
         <v>195</v>
       </c>
       <c r="CB39" t="s">
-        <v>208</v>
+        <v>201</v>
+      </c>
+      <c r="CC39">
+        <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:80">
+    <row r="40" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -10531,10 +10757,13 @@
         <v>195</v>
       </c>
       <c r="CB40" t="s">
-        <v>210</v>
+        <v>203</v>
+      </c>
+      <c r="CC40">
+        <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:80">
+    <row r="41" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -10770,10 +10999,13 @@
         <v>195</v>
       </c>
       <c r="CB41" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC41">
+        <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:80">
+    <row r="42" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -11009,10 +11241,13 @@
         <v>195</v>
       </c>
       <c r="CB42" t="s">
-        <v>211</v>
+        <v>204</v>
+      </c>
+      <c r="CC42">
+        <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:80">
+    <row r="43" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -11124,8 +11359,8 @@
       <c r="AK43">
         <v>500</v>
       </c>
-      <c r="AL43" t="s">
-        <v>202</v>
+      <c r="AL43">
+        <v>496</v>
       </c>
       <c r="AM43" t="s">
         <v>195</v>
@@ -11248,10 +11483,13 @@
         <v>195</v>
       </c>
       <c r="CB43" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC43">
+        <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:80">
+    <row r="44" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -11486,8 +11724,11 @@
       <c r="CA44" t="s">
         <v>195</v>
       </c>
+      <c r="CC44">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:80">
+    <row r="45" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -11645,7 +11886,7 @@
         <v>19</v>
       </c>
       <c r="BA45" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB45">
         <v>22</v>
@@ -11726,10 +11967,13 @@
         <v>195</v>
       </c>
       <c r="CB45" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC45">
+        <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:80">
+    <row r="46" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -11965,10 +12209,13 @@
         <v>195</v>
       </c>
       <c r="CB46" t="s">
-        <v>211</v>
+        <v>204</v>
+      </c>
+      <c r="CC46">
+        <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:80">
+    <row r="47" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -12203,8 +12450,11 @@
       <c r="CA47" t="s">
         <v>195</v>
       </c>
+      <c r="CC47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:80">
+    <row r="48" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -12440,10 +12690,13 @@
         <v>195</v>
       </c>
       <c r="CB48" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC48">
+        <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:80">
+    <row r="49" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -12679,10 +12932,13 @@
         <v>195</v>
       </c>
       <c r="CB49" t="s">
-        <v>212</v>
+        <v>205</v>
+      </c>
+      <c r="CC49">
+        <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:80">
+    <row r="50" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -12917,8 +13173,11 @@
       <c r="CA50" t="s">
         <v>195</v>
       </c>
+      <c r="CC50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:80">
+    <row r="51" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -13076,7 +13335,7 @@
         <v>20</v>
       </c>
       <c r="BA51" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB51">
         <v>20</v>
@@ -13156,8 +13415,11 @@
       <c r="CA51" t="s">
         <v>195</v>
       </c>
+      <c r="CC51">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:80">
+    <row r="52" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -13393,10 +13655,13 @@
         <v>195</v>
       </c>
       <c r="CB52" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC52">
+        <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:80">
+    <row r="53" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -13631,8 +13896,11 @@
       <c r="CA53" t="s">
         <v>195</v>
       </c>
+      <c r="CC53">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:80">
+    <row r="54" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -13790,7 +14058,7 @@
         <v>22</v>
       </c>
       <c r="BA54" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB54">
         <v>21</v>
@@ -13870,8 +14138,11 @@
       <c r="CA54" t="s">
         <v>195</v>
       </c>
+      <c r="CC54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:80">
+    <row r="55" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -14107,10 +14378,13 @@
         <v>195</v>
       </c>
       <c r="CB55" t="s">
-        <v>210</v>
+        <v>203</v>
+      </c>
+      <c r="CC55">
+        <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:80">
+    <row r="56" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -14345,8 +14619,11 @@
       <c r="CA56" t="s">
         <v>195</v>
       </c>
+      <c r="CC56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:80">
+    <row r="57" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -14395,6 +14672,9 @@
       <c r="Q57">
         <v>39</v>
       </c>
+      <c r="R57">
+        <v>416</v>
+      </c>
       <c r="S57" t="s">
         <v>195</v>
       </c>
@@ -14576,10 +14856,13 @@
         <v>195</v>
       </c>
       <c r="CB57" t="s">
-        <v>213</v>
+        <v>206</v>
+      </c>
+      <c r="CC57">
+        <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:80">
+    <row r="58" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -14814,8 +15097,11 @@
       <c r="CA58" t="s">
         <v>195</v>
       </c>
+      <c r="CC58">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:80">
+    <row r="59" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -14973,7 +15259,7 @@
         <v>21</v>
       </c>
       <c r="BA59" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB59">
         <v>20</v>
@@ -15045,16 +15331,20 @@
         <v>488</v>
       </c>
       <c r="BY59">
+        <v>409</v>
+      </c>
+      <c r="BZ59">
+        <f>SUM(BX59,BY59)</f>
+        <v>897</v>
+      </c>
+      <c r="CA59" t="s">
+        <v>195</v>
+      </c>
+      <c r="CC59">
         <v>0</v>
       </c>
-      <c r="BZ59">
-        <v>488</v>
-      </c>
-      <c r="CA59" t="s">
-        <v>195</v>
-      </c>
     </row>
-    <row r="60" spans="1:80">
+    <row r="60" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -15290,10 +15580,13 @@
         <v>195</v>
       </c>
       <c r="CB60" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC60">
+        <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:80">
+    <row r="61" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -15528,8 +15821,11 @@
       <c r="CA61" t="s">
         <v>195</v>
       </c>
+      <c r="CC61">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:80">
+    <row r="62" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -15764,8 +16060,11 @@
       <c r="CA62" t="s">
         <v>195</v>
       </c>
+      <c r="CC62">
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:80">
+    <row r="63" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -16001,10 +16300,13 @@
         <v>195</v>
       </c>
       <c r="CB63" t="s">
-        <v>210</v>
+        <v>203</v>
+      </c>
+      <c r="CC63">
+        <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:80">
+    <row r="64" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -16239,8 +16541,11 @@
       <c r="CA64" t="s">
         <v>195</v>
       </c>
+      <c r="CC64">
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:80">
+    <row r="65" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -16392,7 +16697,7 @@
         <v>20</v>
       </c>
       <c r="BA65" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB65">
         <v>20</v>
@@ -16472,8 +16777,11 @@
       <c r="CA65" t="s">
         <v>195</v>
       </c>
+      <c r="CC65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:80">
+    <row r="66" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -16708,8 +17016,11 @@
       <c r="CA66" t="s">
         <v>195</v>
       </c>
+      <c r="CC66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:80">
+    <row r="67" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -16758,6 +17069,9 @@
       <c r="Q67">
         <v>37</v>
       </c>
+      <c r="R67">
+        <v>420</v>
+      </c>
       <c r="S67" t="s">
         <v>195</v>
       </c>
@@ -16861,7 +17175,7 @@
         <v>19</v>
       </c>
       <c r="BA67" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB67">
         <v>18</v>
@@ -16941,8 +17255,11 @@
       <c r="CA67" t="s">
         <v>195</v>
       </c>
+      <c r="CC67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:80">
+    <row r="68" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -17100,7 +17417,7 @@
         <v>19</v>
       </c>
       <c r="BA68" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB68">
         <v>17</v>
@@ -17180,8 +17497,11 @@
       <c r="CA68" t="s">
         <v>195</v>
       </c>
+      <c r="CC68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:80">
+    <row r="69" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -17417,10 +17737,13 @@
         <v>195</v>
       </c>
       <c r="CB69" t="s">
-        <v>214</v>
+        <v>207</v>
+      </c>
+      <c r="CC69">
+        <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:80">
+    <row r="70" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -17656,10 +17979,13 @@
         <v>195</v>
       </c>
       <c r="CB70" t="s">
-        <v>215</v>
+        <v>208</v>
+      </c>
+      <c r="CC70">
+        <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:80">
+    <row r="71" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -17817,7 +18143,7 @@
         <v>18</v>
       </c>
       <c r="BA71" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB71">
         <v>18</v>
@@ -17897,8 +18223,11 @@
       <c r="CA71" t="s">
         <v>194</v>
       </c>
+      <c r="CC71">
+        <v>0</v>
+      </c>
     </row>
-    <row r="72" spans="1:80">
+    <row r="72" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -18131,10 +18460,13 @@
         <v>194</v>
       </c>
       <c r="CB72" t="s">
-        <v>205</v>
+        <v>198</v>
+      </c>
+      <c r="CC72">
+        <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:80">
+    <row r="73" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -18183,6 +18515,9 @@
       <c r="Q73">
         <v>40</v>
       </c>
+      <c r="R73">
+        <v>437</v>
+      </c>
       <c r="S73" t="s">
         <v>195</v>
       </c>
@@ -18286,7 +18621,7 @@
         <v>22</v>
       </c>
       <c r="BA73" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB73">
         <v>19</v>
@@ -18367,10 +18702,13 @@
         <v>195</v>
       </c>
       <c r="CB73" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC73">
+        <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:80">
+    <row r="74" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -18528,7 +18866,7 @@
         <v>19</v>
       </c>
       <c r="BA74" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB74">
         <v>18</v>
@@ -18609,10 +18947,13 @@
         <v>195</v>
       </c>
       <c r="CB74" t="s">
-        <v>216</v>
+        <v>209</v>
+      </c>
+      <c r="CC74">
+        <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:80">
+    <row r="75" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -18847,8 +19188,11 @@
       <c r="CA75" t="s">
         <v>195</v>
       </c>
+      <c r="CC75">
+        <v>0</v>
+      </c>
     </row>
-    <row r="76" spans="1:80">
+    <row r="76" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -19006,7 +19350,7 @@
         <v>22</v>
       </c>
       <c r="BA76" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB76">
         <v>18</v>
@@ -19086,8 +19430,11 @@
       <c r="CA76" t="s">
         <v>195</v>
       </c>
+      <c r="CC76">
+        <v>0</v>
+      </c>
     </row>
-    <row r="77" spans="1:80">
+    <row r="77" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -19245,7 +19592,7 @@
         <v>23</v>
       </c>
       <c r="BA77" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB77">
         <v>20</v>
@@ -19325,8 +19672,11 @@
       <c r="CA77" t="s">
         <v>195</v>
       </c>
+      <c r="CC77">
+        <v>0</v>
+      </c>
     </row>
-    <row r="78" spans="1:80">
+    <row r="78" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -19484,7 +19834,7 @@
         <v>22</v>
       </c>
       <c r="BA78" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB78">
         <v>22</v>
@@ -19564,8 +19914,11 @@
       <c r="CA78" t="s">
         <v>195</v>
       </c>
+      <c r="CC78">
+        <v>0</v>
+      </c>
     </row>
-    <row r="79" spans="1:80">
+    <row r="79" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -19800,8 +20153,11 @@
       <c r="CA79" t="s">
         <v>195</v>
       </c>
+      <c r="CC79">
+        <v>0</v>
+      </c>
     </row>
-    <row r="80" spans="1:80">
+    <row r="80" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -19853,6 +20209,9 @@
       <c r="Q80">
         <v>34</v>
       </c>
+      <c r="R80">
+        <v>423</v>
+      </c>
       <c r="S80" t="s">
         <v>195</v>
       </c>
@@ -19956,7 +20315,7 @@
         <v>16</v>
       </c>
       <c r="BA80" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB80">
         <v>18</v>
@@ -20036,8 +20395,11 @@
       <c r="CA80" t="s">
         <v>195</v>
       </c>
+      <c r="CC80">
+        <v>0</v>
+      </c>
     </row>
-    <row r="81" spans="1:80">
+    <row r="81" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -20272,8 +20634,11 @@
       <c r="CA81" t="s">
         <v>195</v>
       </c>
+      <c r="CC81">
+        <v>0</v>
+      </c>
     </row>
-    <row r="82" spans="1:80">
+    <row r="82" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -20509,10 +20874,13 @@
         <v>195</v>
       </c>
       <c r="CB82" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC82">
+        <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:80">
+    <row r="83" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -20748,10 +21116,13 @@
         <v>195</v>
       </c>
       <c r="CB83" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC83">
+        <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:80">
+    <row r="84" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -20986,8 +21357,11 @@
       <c r="CA84" t="s">
         <v>195</v>
       </c>
+      <c r="CC84">
+        <v>0</v>
+      </c>
     </row>
-    <row r="85" spans="1:80">
+    <row r="85" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -21222,8 +21596,11 @@
       <c r="CA85" t="s">
         <v>195</v>
       </c>
+      <c r="CC85">
+        <v>0</v>
+      </c>
     </row>
-    <row r="86" spans="1:80">
+    <row r="86" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -21381,7 +21758,7 @@
         <v>20</v>
       </c>
       <c r="BA86" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB86">
         <v>19</v>
@@ -21461,8 +21838,11 @@
       <c r="CA86" t="s">
         <v>195</v>
       </c>
+      <c r="CC86">
+        <v>0</v>
+      </c>
     </row>
-    <row r="87" spans="1:80">
+    <row r="87" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -21698,10 +22078,13 @@
         <v>195</v>
       </c>
       <c r="CB87" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC87">
+        <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:80">
+    <row r="88" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -21937,10 +22320,13 @@
         <v>195</v>
       </c>
       <c r="CB88" t="s">
-        <v>215</v>
+        <v>208</v>
+      </c>
+      <c r="CC88">
+        <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:80">
+    <row r="89" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -22176,10 +22562,13 @@
         <v>195</v>
       </c>
       <c r="CB89" t="s">
-        <v>211</v>
+        <v>204</v>
+      </c>
+      <c r="CC89">
+        <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:80">
+    <row r="90" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -22414,8 +22803,11 @@
       <c r="CA90" t="s">
         <v>195</v>
       </c>
+      <c r="CC90">
+        <v>0</v>
+      </c>
     </row>
-    <row r="91" spans="1:80">
+    <row r="91" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -22650,8 +23042,11 @@
       <c r="CA91" t="s">
         <v>195</v>
       </c>
+      <c r="CC91">
+        <v>0</v>
+      </c>
     </row>
-    <row r="92" spans="1:80">
+    <row r="92" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -22886,8 +23281,11 @@
       <c r="CA92" t="s">
         <v>195</v>
       </c>
+      <c r="CC92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:80">
+    <row r="93" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -23123,10 +23521,13 @@
         <v>195</v>
       </c>
       <c r="CB93" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC93">
+        <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:80">
+    <row r="94" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -23362,10 +23763,13 @@
         <v>195</v>
       </c>
       <c r="CB94" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC94">
+        <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:80">
+    <row r="95" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -23600,8 +24004,11 @@
       <c r="CA95" t="s">
         <v>195</v>
       </c>
+      <c r="CC95">
+        <v>0</v>
+      </c>
     </row>
-    <row r="96" spans="1:80">
+    <row r="96" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -23837,10 +24244,13 @@
         <v>195</v>
       </c>
       <c r="CB96" t="s">
-        <v>205</v>
+        <v>198</v>
+      </c>
+      <c r="CC96">
+        <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:80">
+    <row r="97" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -23998,7 +24408,7 @@
         <v>19</v>
       </c>
       <c r="BA97" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB97">
         <v>19</v>
@@ -24079,10 +24489,13 @@
         <v>194</v>
       </c>
       <c r="CB97" t="s">
-        <v>217</v>
+        <v>210</v>
+      </c>
+      <c r="CC97">
+        <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:80">
+    <row r="98" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -24317,8 +24730,11 @@
       <c r="CA98" t="s">
         <v>195</v>
       </c>
+      <c r="CC98">
+        <v>0</v>
+      </c>
     </row>
-    <row r="99" spans="1:80">
+    <row r="99" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -24554,10 +24970,13 @@
         <v>195</v>
       </c>
       <c r="CB99" t="s">
-        <v>218</v>
+        <v>211</v>
+      </c>
+      <c r="CC99">
+        <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:80">
+    <row r="100" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -24790,10 +25209,13 @@
         <v>195</v>
       </c>
       <c r="CB100" t="s">
-        <v>212</v>
+        <v>205</v>
+      </c>
+      <c r="CC100">
+        <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:80">
+    <row r="101" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -25029,10 +25451,13 @@
         <v>195</v>
       </c>
       <c r="CB101" t="s">
-        <v>205</v>
+        <v>198</v>
+      </c>
+      <c r="CC101">
+        <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:80">
+    <row r="102" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -25268,10 +25693,13 @@
         <v>195</v>
       </c>
       <c r="CB102" t="s">
-        <v>211</v>
+        <v>204</v>
+      </c>
+      <c r="CC102">
+        <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:80">
+    <row r="103" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -25507,10 +25935,13 @@
         <v>195</v>
       </c>
       <c r="CB103" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC103">
+        <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:80">
+    <row r="104" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -25745,8 +26176,11 @@
       <c r="CA104" t="s">
         <v>195</v>
       </c>
+      <c r="CC104">
+        <v>0</v>
+      </c>
     </row>
-    <row r="105" spans="1:80">
+    <row r="105" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -25904,7 +26338,7 @@
         <v>20</v>
       </c>
       <c r="BA105" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB105">
         <v>20</v>
@@ -25984,8 +26418,11 @@
       <c r="CA105" t="s">
         <v>195</v>
       </c>
+      <c r="CC105">
+        <v>0</v>
+      </c>
     </row>
-    <row r="106" spans="1:80">
+    <row r="106" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -26143,7 +26580,7 @@
         <v>22</v>
       </c>
       <c r="BA106" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB106">
         <v>20</v>
@@ -26224,10 +26661,13 @@
         <v>194</v>
       </c>
       <c r="CB106" t="s">
-        <v>219</v>
+        <v>212</v>
+      </c>
+      <c r="CC106">
+        <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:80">
+    <row r="107" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -26385,7 +26825,7 @@
         <v>20</v>
       </c>
       <c r="BA107" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB107">
         <v>20</v>
@@ -26465,8 +26905,11 @@
       <c r="CA107" t="s">
         <v>195</v>
       </c>
+      <c r="CC107">
+        <v>0</v>
+      </c>
     </row>
-    <row r="108" spans="1:80">
+    <row r="108" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -26702,10 +27145,13 @@
         <v>195</v>
       </c>
       <c r="CB108" t="s">
-        <v>210</v>
+        <v>203</v>
+      </c>
+      <c r="CC108">
+        <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:80">
+    <row r="109" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -26940,8 +27386,11 @@
       <c r="CA109" t="s">
         <v>195</v>
       </c>
+      <c r="CC109">
+        <v>0</v>
+      </c>
     </row>
-    <row r="110" spans="1:80">
+    <row r="110" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -27099,7 +27548,7 @@
         <v>18</v>
       </c>
       <c r="BA110" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB110">
         <v>18</v>
@@ -27179,8 +27628,11 @@
       <c r="CA110" t="s">
         <v>195</v>
       </c>
+      <c r="CC110">
+        <v>0</v>
+      </c>
     </row>
-    <row r="111" spans="1:80">
+    <row r="111" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -27415,8 +27867,11 @@
       <c r="CA111" t="s">
         <v>195</v>
       </c>
+      <c r="CC111">
+        <v>0</v>
+      </c>
     </row>
-    <row r="112" spans="1:80">
+    <row r="112" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -27651,8 +28106,11 @@
       <c r="CA112" t="s">
         <v>195</v>
       </c>
+      <c r="CC112">
+        <v>0</v>
+      </c>
     </row>
-    <row r="113" spans="1:80">
+    <row r="113" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -27810,7 +28268,7 @@
         <v>24</v>
       </c>
       <c r="BA113" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB113">
         <v>23</v>
@@ -27891,10 +28349,13 @@
         <v>195</v>
       </c>
       <c r="CB113" t="s">
-        <v>205</v>
+        <v>198</v>
+      </c>
+      <c r="CC113">
+        <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:80">
+    <row r="114" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -28052,7 +28513,7 @@
         <v>15</v>
       </c>
       <c r="BA114" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BB114">
         <v>20</v>
@@ -28132,8 +28593,11 @@
       <c r="CA114" t="s">
         <v>195</v>
       </c>
+      <c r="CC114">
+        <v>0</v>
+      </c>
     </row>
-    <row r="115" spans="1:80">
+    <row r="115" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -28369,10 +28833,13 @@
         <v>195</v>
       </c>
       <c r="CB115" t="s">
-        <v>206</v>
+        <v>199</v>
+      </c>
+      <c r="CC115">
+        <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:80">
+    <row r="116" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -28567,9 +29034,13 @@
       </c>
       <c r="CA116" t="s">
         <v>195</v>
+      </c>
+      <c r="CC116">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>